<commit_message>
final implementation prep & repo cleanup
</commit_message>
<xml_diff>
--- a/app/lib/appDriversAndFormulas_v.1.2.xlsx
+++ b/app/lib/appDriversAndFormulas_v.1.2.xlsx
@@ -2557,11 +2557,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1166707696"/>
-        <c:axId val="-1170518880"/>
+        <c:axId val="-797412800"/>
+        <c:axId val="-797408416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1166707696"/>
+        <c:axId val="-797412800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2599,7 +2599,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1170518880"/>
+        <c:crossAx val="-797408416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2607,7 +2607,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1170518880"/>
+        <c:axId val="-797408416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2641,7 +2641,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1166707696"/>
+        <c:crossAx val="-797412800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -33727,8 +33727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="K56" sqref="K56"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelRow="2" x14ac:dyDescent="0.2"/>

</xml_diff>